<commit_message>
NOAA GHCND FINISHED BY GEMINI FROM GOOGLE AI STUDIO
</commit_message>
<xml_diff>
--- a/气象/蒙古存档.xlsx
+++ b/气象/蒙古存档.xlsx
@@ -11399,49 +11399,88 @@
       <c r="A240" s="1" t="n">
         <v>45999</v>
       </c>
-      <c r="B240" t="n">
+      <c r="B240" s="0" t="n">
         <v>-21.1</v>
       </c>
-      <c r="C240" t="n">
+      <c r="C240" s="0" t="n">
         <v>-26.4</v>
       </c>
-      <c r="D240" t="n">
+      <c r="D240" s="0" t="n">
         <v>-24.7</v>
       </c>
-      <c r="E240" t="n">
+      <c r="E240" s="0" t="n">
         <v>-25.3</v>
       </c>
-      <c r="F240" t="n">
+      <c r="F240" s="0" t="n">
         <v>-32.5</v>
       </c>
-      <c r="G240" t="n">
+      <c r="G240" s="0" t="n">
         <v>-23</v>
       </c>
-      <c r="H240" t="n">
+      <c r="H240" s="0" t="n">
         <v>-26.8</v>
       </c>
-      <c r="I240" t="n">
+      <c r="I240" s="0" t="n">
         <v>-23.6</v>
       </c>
-      <c r="J240" t="n">
+      <c r="J240" s="0" t="n">
         <v>-24.2</v>
       </c>
-      <c r="K240" t="n">
+      <c r="K240" s="0" t="n">
         <v>-19.9</v>
       </c>
-      <c r="L240" t="n">
+      <c r="L240" s="0" t="n">
         <v>-29.3</v>
       </c>
-      <c r="M240" t="n">
+      <c r="M240" s="0" t="n">
         <v>-27.5</v>
       </c>
-      <c r="N240" t="n">
+      <c r="N240" s="0" t="n">
         <v>-22.6</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
         <v>46000</v>
+      </c>
+      <c r="B241" t="n">
+        <v>-20.1</v>
+      </c>
+      <c r="C241" t="n">
+        <v>-25.7</v>
+      </c>
+      <c r="D241" t="n">
+        <v>-25.8</v>
+      </c>
+      <c r="E241" t="n">
+        <v>-24.2</v>
+      </c>
+      <c r="F241" t="n">
+        <v>-30.2</v>
+      </c>
+      <c r="G241" t="n">
+        <v>-19.5</v>
+      </c>
+      <c r="H241" t="n">
+        <v>-26.6</v>
+      </c>
+      <c r="I241" t="n">
+        <v>-23.2</v>
+      </c>
+      <c r="J241" t="n">
+        <v>-25.8</v>
+      </c>
+      <c r="K241" t="n">
+        <v>-23.9</v>
+      </c>
+      <c r="L241" t="n">
+        <v>-24.8</v>
+      </c>
+      <c r="M241" t="n">
+        <v>-24.9</v>
+      </c>
+      <c r="N241" t="n">
+        <v>-20.8</v>
       </c>
     </row>
     <row r="242">
@@ -22913,49 +22952,88 @@
       <c r="A240" s="1" t="n">
         <v>45999</v>
       </c>
-      <c r="B240" t="n">
+      <c r="B240" s="0" t="n">
         <v>-14</v>
       </c>
-      <c r="C240" t="n">
+      <c r="C240" s="0" t="n">
         <v>-18.2</v>
       </c>
-      <c r="D240" t="n">
+      <c r="D240" s="0" t="n">
         <v>-12.8</v>
       </c>
-      <c r="E240" t="n">
+      <c r="E240" s="0" t="n">
         <v>-11.5</v>
       </c>
-      <c r="F240" t="n">
+      <c r="F240" s="0" t="n">
         <v>-19.6</v>
       </c>
-      <c r="G240" t="n">
+      <c r="G240" s="0" t="n">
         <v>-16.9</v>
       </c>
-      <c r="H240" t="n">
+      <c r="H240" s="0" t="n">
         <v>-16.3</v>
       </c>
-      <c r="I240" t="n">
+      <c r="I240" s="0" t="n">
         <v>-13.5</v>
       </c>
-      <c r="J240" t="n">
+      <c r="J240" s="0" t="n">
         <v>-13.9</v>
       </c>
-      <c r="K240" t="n">
+      <c r="K240" s="0" t="n">
         <v>-7.1</v>
       </c>
-      <c r="L240" t="n">
+      <c r="L240" s="0" t="n">
         <v>-10.2</v>
       </c>
-      <c r="M240" t="n">
+      <c r="M240" s="0" t="n">
         <v>-15.5</v>
       </c>
-      <c r="N240" t="n">
+      <c r="N240" s="0" t="n">
         <v>-10.8</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
         <v>46000</v>
+      </c>
+      <c r="B241" t="n">
+        <v>-15.1</v>
+      </c>
+      <c r="C241" t="n">
+        <v>-14.7</v>
+      </c>
+      <c r="D241" t="n">
+        <v>-15.8</v>
+      </c>
+      <c r="E241" t="n">
+        <v>-14.3</v>
+      </c>
+      <c r="F241" t="n">
+        <v>-17.4</v>
+      </c>
+      <c r="G241" t="n">
+        <v>-15.9</v>
+      </c>
+      <c r="H241" t="n">
+        <v>-20</v>
+      </c>
+      <c r="I241" t="n">
+        <v>-12.5</v>
+      </c>
+      <c r="J241" t="n">
+        <v>-16.7</v>
+      </c>
+      <c r="K241" t="n">
+        <v>-10.1</v>
+      </c>
+      <c r="L241" t="n">
+        <v>-14.2</v>
+      </c>
+      <c r="M241" t="n">
+        <v>-15.7</v>
+      </c>
+      <c r="N241" t="n">
+        <v>-14.3</v>
       </c>
     </row>
     <row r="242">

</xml_diff>